<commit_message>
updated employee billing utilization
</commit_message>
<xml_diff>
--- a/Content/ExcelTemplates/CBS_EmployeeBillingUtilization.xlsx
+++ b/Content/ExcelTemplates/CBS_EmployeeBillingUtilization.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Employee Name</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>EmpID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">company / Initiative utilization </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilization on self </t>
   </si>
 </sst>
 </file>
@@ -75,9 +81,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,10 +404,12 @@
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +425,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>